<commit_message>
remove eu from urn:iso:std:iso:3166
</commit_message>
<xml_diff>
--- a/ePICreator/Humalog.xlsx
+++ b/ePICreator/Humalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/vulcan-eproduct-info/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4AB65-10E7-1640-B0EB-9B391F27EF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F8D5C5-0BB7-914D-830F-A73B72D2CD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="AdministrableProductDefinition" sheetId="1" r:id="rId1"/>
@@ -656,12 +656,6 @@
     </r>
   </si>
   <si>
-    <t>eu</t>
-  </si>
-  <si>
-    <t>European Union</t>
-  </si>
-  <si>
     <r>
       <t>ORG</t>
     </r>
@@ -1120,6 +1114,12 @@
   </si>
   <si>
     <t>address_postalCode</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>DK</t>
   </si>
 </sst>
 </file>
@@ -1549,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A7762C-AB2F-B34F-B02E-3A163776DCB2}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>98</v>
@@ -1765,10 +1765,10 @@
         <v>119</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1907,10 +1907,10 @@
     <row r="2" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>53</v>
@@ -1923,26 +1923,26 @@
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>96</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2120,7 +2120,7 @@
         <v>100</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -2271,7 +2271,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:W1"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2316,13 +2316,13 @@
         <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
@@ -2352,13 +2352,13 @@
         <v>69</v>
       </c>
       <c r="T1" t="s">
+        <v>164</v>
+      </c>
+      <c r="U1" t="s">
+        <v>165</v>
+      </c>
+      <c r="V1" t="s">
         <v>166</v>
-      </c>
-      <c r="U1" t="s">
-        <v>167</v>
-      </c>
-      <c r="V1" t="s">
-        <v>168</v>
       </c>
       <c r="W1" t="s">
         <v>10</v>
@@ -2367,34 +2367,34 @@
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="9">
         <v>123456</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" t="s">
         <v>151</v>
       </c>
-      <c r="F2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G2" t="s">
-        <v>153</v>
-      </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="J2" t="s">
         <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L2" t="s">
         <v>8</v>
@@ -2430,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1B07EB-5F76-7E4B-ABAA-4F88BE5E2A71}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2477,7 +2477,7 @@
         <v>75</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -2486,10 +2486,10 @@
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -2501,7 +2501,7 @@
         <v>220000000034</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
@@ -2510,33 +2510,33 @@
         <v>33</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" t="s">
         <v>129</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="L2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F3" s="9">
         <v>220000000033</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
         <v>32</v>
@@ -2545,33 +2545,33 @@
         <v>33</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="L3" t="s">
         <v>136</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="L3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D4" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F4" s="9">
         <v>220000000033</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -2580,13 +2580,13 @@
         <v>33</v>
       </c>
       <c r="J4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2669,7 +2669,7 @@
         <v>39</v>
       </c>
       <c r="P1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q1" t="s">
         <v>10</v>
@@ -2727,7 +2727,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2774,7 +2774,7 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>119</v>
@@ -2795,10 +2795,10 @@
         <v>100000072062</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added draft por focused
</commit_message>
<xml_diff>
--- a/ePICreator/Humalog.xlsx
+++ b/ePICreator/Humalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/vulcan-eproduct-info/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D724D2F-E53A-974A-B435-B5895F8B671E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45684C8B-8D3A-8349-992C-4F7249547732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
@@ -1262,30 +1262,10 @@
 dispose of medicines no longer required. These measures will help to protect the environment.&lt;/p&gt;        &lt;/div&gt;</t>
   </si>
   <si>
-    <r>
-      <t>EU</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/1/96/007/035</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>|0xF79CABF272B6A7EEF104DDDA44E82717</t>
-    </r>
-  </si>
-  <si>
     <t>https://spor.ema.europa.eu/pmswi|https://www.who-umc.org/phpid</t>
+  </si>
+  <si>
+    <t>EU/1/96/007/035|0xF79CABF272B6A7EEF104DDDA44E82717</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2484,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C4:C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2590,10 +2570,10 @@
         <v>133</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
correct template and some issues on humalog
</commit_message>
<xml_diff>
--- a/ePICreator/Humalog.xlsx
+++ b/ePICreator/Humalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/vulcan-eproduct-info/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45684C8B-8D3A-8349-992C-4F7249547732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDD969E-988F-EA41-8538-01A63CA7043E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="AdministrableProductDefinition" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="174">
   <si>
     <t>id</t>
   </si>
@@ -310,83 +310,6 @@
   </si>
   <si>
     <t>other_info</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Humalog </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ml </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> pre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>filled pen</t>
-    </r>
   </si>
   <si>
     <t>0x073AF2E5B92AE19E8B67635AFFB3D6CA</t>
@@ -480,101 +403,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Humalog </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> units</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ml KwikPen solution </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>for</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> injection </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a pre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>filled pen</t>
-    </r>
-  </si>
-  <si>
     <t>3 ml</t>
   </si>
   <si>
@@ -878,29 +706,6 @@
   </si>
   <si>
     <t>ES</t>
-  </si>
-  <si>
-    <r>
-      <t>Humalog Mix50 Insulin KwikPen, 3ml pre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9D1D9"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>fill</t>
-    </r>
   </si>
   <si>
     <t>country</t>
@@ -942,19 +747,6 @@
   </si>
   <si>
     <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
-&lt;b&gt;6. Contents of the pack and other information&lt;/b&gt;
-&lt;b&gt;What Humalog Mix50 100 units/ml suspension for injection in cartridge contains&lt;/b&gt;
-&lt;p&gt;The active substance is insulin lispro. Insulin lispro is made in the laboratory by a ‘recombinant
-DNA technology’ process. It is a changed form of human insulin and so is different from other
-human and animal insulins. Insulin lispro is closely related to human insulin which is a natural
-hormone made by the pancreas.
-The other ingredients are protamine sulphate, m-cresol, phenol, glycerol, dibasic sodium
-phosphate 7H2O, zinc oxide and water for injection. Sodium hydroxide or hydrochloric acid
-may have been used to adjust the acidity.&lt;/p&gt;
-&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
 What in this leaflet
 &lt;ol&gt;
   &lt;li&gt;What Humalog Mix50 is and what it is used for&lt;/li&gt;
@@ -967,12 +759,6 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
-&lt;p&gt;&lt;b&gt;4. Possible side effects&lt;/b&gt;&lt;/p&gt;
-&lt;p&gt;Like all medicines, this medicine can cause side effects, although not everybody gets them.&lt;/p&gt;
-&lt;/div&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Humalog </t>
   </si>
   <si>
@@ -1060,86 +846,6 @@
   </si>
   <si>
     <t>xx</t>
-  </si>
-  <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
-&lt;b&gt;2. What you need to know before you use Humalog Mix50&lt;/b&gt;
-&lt;p&gt;&lt;strong&gt;Do NOT use Humalog Mix50&lt;/strong&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;if you think hypoglycaemia (low blood sugar) is starting. Further in this leaflet it tells you how to
-deal with mild hypoglycaemia (see Section 3: If you take more Humalog Mix50 than you need).&lt;/li&gt;
-&lt;li&gt;if you are allergic to insulin lispro or any of the other ingredients of this medicine (listed in
-section 6).&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;strong&gt;Warnings and precautions&lt;/strong&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Always check the pack and the cartridge label for the name and type of the insulin when you get
-it from your pharmacy. Make sure you get the Humalog Mix50 that your doctor has told you to
-use.&lt;/li&gt;
-&lt;li&gt;If your blood sugar levels are well controlled by your current insulin therapy, you may not feel the
-warning symptoms when your blood sugar is falling too low. Warning signs are listed later in this
-leaflet. You must think carefully about when to have your meals, how often to exercise and how much to do. You must also keep a close watch on your blood sugar levels by testing your blood
-glucose often.&lt;/li&gt;
-&lt;li&gt;A few people who have had hypoglycaemia after switching from animal insulin to human insulin
-have reported that the early warning symptoms were less obvious or different. If you often have
-hypoglycaemia or have difficulty recognising them, please discuss this with your doctor.&lt;/li&gt;
-&lt;li&gt;If you answer YES to any of the following questions, tell your doctor, pharmacist or diabetes
-nurse&lt;ul&gt;
-&lt;li&gt;Have you recently become ill?&lt;/li&gt;
-&lt;li&gt;Do you have trouble with your kidneys or liver?&lt;/li&gt;
-&lt;li&gt;Are you exercising more than usual?&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/li&gt;
-&lt;li&gt;The amount of insulin you need may also change if you drink alcohol.&lt;/li&gt;
-&lt;li&gt;You should also tell your doctor, pharmacist or diabetes nurse if you are planning to go abroad.
-The time difference between countries may mean that you have to have your injections and meals
-at different times from when you are at home.&lt;/li&gt;
-&lt;li&gt;Some patients with long-standing type 2 diabetes mellitus and heart disease or previous stroke
-who were treated with pioglitazone and insulin experienced the development of heart failure.
-Inform your doctor as soon as possible, if you experience signs of heart failure such as unusual
-shortness of breath or rapid increase in weight or localised swelling (oedema).&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;strong&gt;Skin changes at the injection site&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;The injection site should be rotated to prevent skin changes such as lumps under the skin. The insulin
-may not work very well if you inject into a lumpy area (See How to use Humalog Mix50). Contact
-your doctor if you are currently injecting into a lumpy area before you start injecting a different area.
-Your doctor may tell you to check your blood sugar more closely, and to adjust your insulin or your other antidiabetic medications dose.&lt;/p&gt;
-&lt;p&gt;&lt;strong&gt;Other medicines and Humalog Mix50&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;Your insulin needs may change if you are taking&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;the contraceptive pill,&lt;/li&gt;
-&lt;li&gt;steroids,&lt;/li&gt;
-&lt;li&gt;thyroid hormone replacement therapy,&lt;/li&gt;
-&lt;li&gt;oral hypoglycaemics,&lt;/li&gt;
-&lt;li&gt;acetyl salicylic acid,&lt;/li&gt;
-&lt;li&gt;sulpha antibiotics,&lt;/li&gt;
-&lt;li&gt;octreotide,&lt;/li&gt;
-&lt;li&gt;“beta2 stimulants” (for example ritodrine, salbutamol or terbutaline),&lt;/li&gt;
-&lt;li&gt;beta-blockers, or&lt;/li&gt;
-&lt;li&gt;some antidepressants (monoamine oxidase inhibitors or selective serotonin reuptake inhibitors),&lt;/li&gt;
-&lt;li&gt;danazol,&lt;/li&gt;
-&lt;li&gt;some angiotensin converting enzyme (ACE) inhibitors (for example captopril, enalapril), and&lt;/li&gt;
-&lt;li&gt;angiotensin II receptor blockers.
-Please tell your doctor, if you are taking, have recently taken or might take any other medicines,
-including medicines obtained without a prescription (see section “Warnings and precautions”).&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;strong&gt;Pregnancy and breast-feeding&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;Are you pregnant or thinking about becoming pregnant, or are you breast-feeding? The amount of
-insulin you need usually falls during the first three months of pregnancy and increases for the
-remaining six months. If you are breast-feeding, you may need to alter your insulin intake or diet.
-Ask your doctor for advice.&lt;/p&gt;
-&lt;p&gt;&lt;strong&gt;Driving and using machines&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;Your ability to concentrate and react may be reduced if you have hypoglycaemia. Please keep this
-possible problem in mind in all situations where you might put yourself and others at risk (e.g. driving
-a car or operating machinery). You should contact your doctor about the advisability of driving if you
-have: &lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;frequent episodes of hypoglycaemia&lt;/li&gt;
-&lt;li&gt;reduced or absent warning signs of hypoglycaemia
-Humalog Mix50 contains sodium
-This medicine contains less than 1 mmol sodium (23 mg) per dose, that is to say essentially ‘sodium-free’.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
@@ -1230,25 +936,101 @@
 &lt;p&gt;If you have any further questions on the use of this product, ask your doctor or pharmacist&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
-&lt;b&gt;1.What Humalog Mix50 is and what it is used for&lt;/b&gt;
-Humalog Mix50 is used to treat diabetes. Humalog Mix50 is a premixed suspension. Its active
-substance is insulin lispro. 50% of the insulin lispro in Humalog Mix50 is dissolved in water and it
-works more quickly than normal human insulin because the insulin molecule has been changed
-slightly. 50% of the insulin lispro in Humalog Mix50 is available in a suspension together with
-protamine sulphate, so that its action is prolonged.
-You get diabetes if your pancreas does not make enough insulin to control the level of glucose in
-your blood. Humalog Mix50 is a substitute for your own insulin and is used to control glucose in the
-long term. Humalog Mix50 works very quickly and longer than soluble insulin. You should
-normally use Humalog Mix50 within 15 minutes of a meal.
-Your doctor may tell you to use Humalog Mix50 as well as a longer-acting insulin. Each kind of
-insulin comes with another patient information leaflet to tell you about it. Do not change your
-insulin unless your doctor tells you to. Be very careful if you do change insulin.
-&lt;/div&gt;</t>
+    <t>https://spor.ema.europa.eu/pmswi|https://www.who-umc.org/phpid</t>
+  </si>
+  <si>
+    <t>EU/1/96/007/035|0xF79CABF272B6A7EEF104DDDA44E82717</t>
+  </si>
+  <si>
+    <t>Humalog Mix50 Insulin KwikPen, 100 U/ml, Suspension for injection 3ml pre-fill</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Humalog is used to treat diabetes. Humalog works more quickly than normal human insulin because
+the insulin molecule has been changed slightly.&lt;/p&gt;
+&lt;p&gt;You get diabetes if your pancreas does not make enough insulin to control the level of glucose in your
+blood. Humalog is a substitute for your own insulin and is used to control glucose in the long term. It
+works very quickly and lasts a shorter time than soluble insulin (2 to 5 hours). You should normally
+use Humalog within 15 minutes of a meal.&lt;/p&gt;
+&lt;p&gt;Your doctor may tell you to use Humalog as well as a longer-acting insulin. Each kind of insulin
+comes with another patient information leaflet to tell you about it. Do not change your insulin unless
+your doctor tells you to. Be very careful if you do change insulin.&lt;/p&gt;
+&lt;p&gt;Humalog is suitable for use in adults and children.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Like all medicines, this medicine can cause side effects, although not everybody gets them.
+Systemic allergy is rare (≥ 1/10,000 to &amp;lt;1/1,000). The symptoms are as follows:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;rash over the whole body&lt;/li&gt;
+&lt;li&gt;blood pressure dropping&lt;/li&gt;
+&lt;li&gt;difficulty in breathing &lt;/li&gt;
+&lt;li&gt;heart beating fast&lt;/li&gt;
+&lt;li&gt;wheezing &lt;/li&gt;
+&lt;li&gt;sweating&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;If you think you are having this sort of insulin allergy with Humalog, tell your doctor at once.&lt;/p&gt;
+&lt;p&gt;Local allergy is common (≥ 1/100 to &amp;lt;1/10). Some people get redness, swelling or itching around the
+area of the insulin injection. This usually clears up in anything from a few days to a few weeks. If this
+happens to you, tell your doctor.&lt;/p&gt;
+&lt;p&gt;Lipodystrophy is uncommon (≥ 1/1,000 to &amp;lt;1/100). If you inject insulin too often at the same place,
+the fatty tissue may either shrink (lipoatrophy) or thicken (lipohypertrophy). Lumps under the skin
+may also be caused by build-up of a protein called amyloid (cutaneous amyloidosis). The insulin may
+not work very well if you inject into a lumpy area. Change the injection site with each injection to help
+prevent these skin changes.&lt;/p&gt;
+&lt;p&gt;Oedema (e.g. swelling in arms, ankles; fluid retention) has been reported, particularly at the start of
+insulin therapy or during a change in therapy to improve control of your blood glucose.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Reporting of side effects&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;If you get any side effects, talk to your doctor or pharmacist. This includes any possible side effects
+not listed in this leaflet. You can also report side effects directly via the national reporting system
+listed in Appendix V. By reporting side effects you can help provide more information on the safety of
+this medicine.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Common problems of diabetes&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;A. Hypoglycaemia&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Hypoglycaemia (low blood sugar) means there is not enough sugar in the blood. This can be caused if:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;you take too much Humalog or other insulin;&lt;/li&gt;
+&lt;li&gt;you miss or delay meals or change your diet;&lt;/li&gt;
+&lt;li&gt;you exercise or work too hard just before or after a meal;&lt;/li&gt;
+&lt;li&gt;you have an infection or illness (especially diarrhoea or vomiting);&lt;/li&gt;
+&lt;li&gt;there is a change in your need for insulin; or&lt;/li&gt;
+&lt;li&gt;you have trouble with your kidneys or liver which gets worse.
+Alcohol and some medicines can affect your blood sugar levels.
+The first symptoms of low blood sugar usually come on quickly and include the following:&lt;/li&gt;
+&lt;li&gt;tiredness &lt;/li&gt;
+&lt;li&gt;rapid heartbeat&lt;/li&gt;
+&lt;li&gt;nervousness or shakiness&lt;/li&gt;
+&lt;li&gt;feeling sick&lt;/li&gt;
+&lt;li&gt;headache&lt;/li&gt;
+&lt;li&gt;cold sweat.
+While you are not confident about recognising your warning symptoms, avoid situations, e.g. driving a
+car, in which you or others would be put at risk by hypoglycaemia.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;B. Hyperglycaemia and diabetic ketoacidosis&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Hyperglycaemia (too much sugar in the blood) means that your body does not have enough insulin.
+Hyperglycaemia can be brought about by:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;not taking your Humalog or other insulin;&lt;/li&gt;
+&lt;li&gt;taking less insulin than your doctor tells you to;&lt;/li&gt;
+&lt;li&gt;eating a lot more than your diet allows; or&lt;/li&gt;
+&lt;li&gt;fever, infection or emotional stress.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hyperglycaemia can lead to diabetic ketoacidosis. The first symptoms come on slowly over many
+hours or days. The symptoms include the following:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;feeling sleepy &lt;/li&gt;
+&lt;li&gt;no appetite&lt;/li&gt;
+&lt;li&gt;flushed face&lt;/li&gt;
+&lt;li&gt;fruity smell on the breath&lt;/li&gt;
+&lt;li&gt;thirst&lt;/li&gt;
+&lt;li&gt;feeling or being sick
+Severe symptoms are heavy breathing and a rapid pulse. &lt;strong&gt;Get medical help immediately.&lt;/strong&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;C. Illness&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;If you are ill, especially if you feel sick or are sick, the amount of insulin you need may change. Even
+when you are not eating normally, you still need insulin. Test your urine or blood, follow your
+‘sick rules’, and tell your doctor.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-&lt;p&gt;&lt;strong&gt;5. How to store Humalog Mix50&lt;/strong&gt;&lt;/p&gt;
 &lt;p&gt;Before the first use store your Humalog Mix50 in a refrigerator (2°C – 8°C). Do not freeze.
 Keep your cartridge in use at room temperature (below 30°C) and discard after 28 days. Do not put it
 near heat or in the sun. Do not keep your pen or the cartridges you are using in the fridge. The pen
@@ -1262,17 +1044,102 @@
 dispose of medicines no longer required. These measures will help to protect the environment.&lt;/p&gt;        &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://spor.ema.europa.eu/pmswi|https://www.who-umc.org/phpid</t>
-  </si>
-  <si>
-    <t>EU/1/96/007/035|0xF79CABF272B6A7EEF104DDDA44E82717</t>
+    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
+&lt;b&gt;What Humalog Mix50 100 units/ml suspension for injection in cartridge contains&lt;/b&gt;
+&lt;p&gt;The active substance is insulin lispro. Insulin lispro is made in the laboratory by a ‘recombinant
+DNA technology’ process. It is a changed form of human insulin and so is different from other
+human and animal insulins. Insulin lispro is closely related to human insulin which is a natural
+hormone made by the pancreas.
+The other ingredients are protamine sulphate, m-cresol, phenol, glycerol, dibasic sodium
+phosphate 7H2O, zinc oxide and water for injection. Sodium hydroxide or hydrochloric acid
+may have been used to adjust the acidity.&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt;
+&lt;p&gt;&lt;strong&gt;Do NOT use Humalog Mix50&lt;/strong&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;if you think hypoglycaemia (low blood sugar) is starting. Further in this leaflet it tells you how to
+deal with mild hypoglycaemia (see Section 3: If you take more Humalog Mix50 than you need).&lt;/li&gt;
+&lt;li&gt;if you are allergic to insulin lispro or any of the other ingredients of this medicine (listed in
+section 6).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Warnings and precautions&lt;/strong&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Always check the pack and the cartridge label for the name and type of the insulin when you get
+it from your pharmacy. Make sure you get the Humalog Mix50 that your doctor has told you to
+use.&lt;/li&gt;
+&lt;li&gt;If your blood sugar levels are well controlled by your current insulin therapy, you may not feel the
+warning symptoms when your blood sugar is falling too low. Warning signs are listed later in this
+leaflet. You must think carefully about when to have your meals, how often to exercise and how much to do. You must also keep a close watch on your blood sugar levels by testing your blood
+glucose often.&lt;/li&gt;
+&lt;li&gt;A few people who have had hypoglycaemia after switching from animal insulin to human insulin
+have reported that the early warning symptoms were less obvious or different. If you often have
+hypoglycaemia or have difficulty recognising them, please discuss this with your doctor.&lt;/li&gt;
+&lt;li&gt;If you answer YES to any of the following questions, tell your doctor, pharmacist or diabetes
+nurse&lt;ul&gt;
+&lt;li&gt;Have you recently become ill?&lt;/li&gt;
+&lt;li&gt;Do you have trouble with your kidneys or liver?&lt;/li&gt;
+&lt;li&gt;Are you exercising more than usual?&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;The amount of insulin you need may also change if you drink alcohol.&lt;/li&gt;
+&lt;li&gt;You should also tell your doctor, pharmacist or diabetes nurse if you are planning to go abroad.
+The time difference between countries may mean that you have to have your injections and meals
+at different times from when you are at home.&lt;/li&gt;
+&lt;li&gt;Some patients with long-standing type 2 diabetes mellitus and heart disease or previous stroke
+who were treated with pioglitazone and insulin experienced the development of heart failure.
+Inform your doctor as soon as possible, if you experience signs of heart failure such as unusual
+shortness of breath or rapid increase in weight or localised swelling (oedema).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Skin changes at the injection site&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;The injection site should be rotated to prevent skin changes such as lumps under the skin. The insulin
+may not work very well if you inject into a lumpy area (See How to use Humalog Mix50). Contact
+your doctor if you are currently injecting into a lumpy area before you start injecting a different area.
+Your doctor may tell you to check your blood sugar more closely, and to adjust your insulin or your other antidiabetic medications dose.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Other medicines and Humalog Mix50&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Your insulin needs may change if you are taking&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;the contraceptive pill,&lt;/li&gt;
+&lt;li&gt;steroids,&lt;/li&gt;
+&lt;li&gt;thyroid hormone replacement therapy,&lt;/li&gt;
+&lt;li&gt;oral hypoglycaemics,&lt;/li&gt;
+&lt;li&gt;acetyl salicylic acid,&lt;/li&gt;
+&lt;li&gt;sulpha antibiotics,&lt;/li&gt;
+&lt;li&gt;octreotide,&lt;/li&gt;
+&lt;li&gt;“beta2 stimulants” (for example ritodrine, salbutamol or terbutaline),&lt;/li&gt;
+&lt;li&gt;beta-blockers, or&lt;/li&gt;
+&lt;li&gt;some antidepressants (monoamine oxidase inhibitors or selective serotonin reuptake inhibitors),&lt;/li&gt;
+&lt;li&gt;danazol,&lt;/li&gt;
+&lt;li&gt;some angiotensin converting enzyme (ACE) inhibitors (for example captopril, enalapril), and&lt;/li&gt;
+&lt;li&gt;angiotensin II receptor blockers.
+Please tell your doctor, if you are taking, have recently taken or might take any other medicines,
+including medicines obtained without a prescription (see section “Warnings and precautions”).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Pregnancy and breast-feeding&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Are you pregnant or thinking about becoming pregnant, or are you breast-feeding? The amount of
+insulin you need usually falls during the first three months of pregnancy and increases for the
+remaining six months. If you are breast-feeding, you may need to alter your insulin intake or diet.
+Ask your doctor for advice.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Driving and using machines&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Your ability to concentrate and react may be reduced if you have hypoglycaemia. Please keep this
+possible problem in mind in all situations where you might put yourself and others at risk (e.g. driving
+a car or operating machinery). You should contact your doctor about the advisability of driving if you
+have: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;frequent episodes of hypoglycaemia&lt;/li&gt;
+&lt;li&gt;reduced or absent warning signs of hypoglycaemia
+Humalog Mix50 contains sodium
+This medicine contains less than 1 mmol sodium (23 mg) per dose, that is to say essentially ‘sodium-free’.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1378,6 +1245,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC3E88D"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1400,7 +1273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1423,6 +1296,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1741,7 +1615,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1798,28 +1672,28 @@
     </row>
     <row r="2" spans="1:13">
       <c r="B2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" t="s">
         <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2">
         <v>100000073864</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2">
         <v>200000002135</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J2">
         <v>100000073633</v>
@@ -1904,26 +1778,26 @@
     <row r="2" spans="1:14" ht="21">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" s="16"/>
       <c r="I2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="L2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1975,10 +1849,10 @@
         <v>42</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2051,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05DE958-7C5A-B14B-9983-3CEB258B5640}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2117,7 +1991,7 @@
     <row r="2" spans="1:16" ht="409.6">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>48</v>
@@ -2133,28 +2007,28 @@
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2228,10 +2102,10 @@
     <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2248,10 +2122,10 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -2268,10 +2142,10 @@
     <row r="4" spans="1:13">
       <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -2288,10 +2162,10 @@
     <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" s="13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -2308,10 +2182,10 @@
     <row r="6" spans="1:13">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -2332,16 +2206,16 @@
         <v>100</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1"/>
       <c r="B7" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -2358,10 +2232,10 @@
     <row r="8" spans="1:13">
       <c r="A8" s="1"/>
       <c r="B8" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -2378,10 +2252,10 @@
     <row r="9" spans="1:13">
       <c r="A9" s="1"/>
       <c r="B9" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -2412,7 +2286,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2453,22 +2327,22 @@
     <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="10">
         <v>100000073864</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" s="9">
         <v>200000002135</v>
@@ -2483,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EB2795-F6E7-D149-BA96-099EC7B435E4}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2531,13 +2405,13 @@
         <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
         <v>25</v>
@@ -2552,13 +2426,13 @@
         <v>60</v>
       </c>
       <c r="P1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="Q1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="R1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="S1" t="s">
         <v>10</v>
@@ -2566,38 +2440,38 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
-        <v>133</v>
+      <c r="B2" s="18" t="s">
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" t="s">
-        <v>140</v>
-      </c>
       <c r="I2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K2" t="s">
         <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M2" t="s">
         <v>8</v>
@@ -2609,10 +2483,10 @@
         <v>100000072084</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2672,7 +2546,7 @@
         <v>66</v>
       </c>
       <c r="M1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -2681,10 +2555,10 @@
     <row r="2" spans="1:14">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -2696,7 +2570,7 @@
         <v>220000000034</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -2705,33 +2579,33 @@
         <v>30</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" t="s">
         <v>116</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="B3" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F3" s="9">
         <v>220000000033</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -2740,33 +2614,33 @@
         <v>30</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" t="s">
         <v>123</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="L3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="B4" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F4" s="9">
         <v>220000000033</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -2775,13 +2649,13 @@
         <v>30</v>
       </c>
       <c r="J4" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2795,7 +2669,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2852,7 +2726,7 @@
         <v>70</v>
       </c>
       <c r="L1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M1" t="s">
         <v>32</v>
@@ -2864,25 +2738,25 @@
         <v>35</v>
       </c>
       <c r="P1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="R1" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="S1" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="V1" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>160</v>
       </c>
       <c r="W1" s="12" t="s">
         <v>10</v>
@@ -2891,10 +2765,10 @@
     <row r="2" spans="1:23">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -2909,13 +2783,13 @@
         <v>100000155527</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I2">
         <v>123456</v>
       </c>
       <c r="J2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K2" s="9">
         <v>100000073543</v>
@@ -2924,7 +2798,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N2" s="9">
         <v>200000003204</v>
@@ -2987,10 +2861,10 @@
     <row r="2" spans="1:11">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -3008,10 +2882,10 @@
         <v>100000072062</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>